<commit_message>
Add new method to RailwayNetwork. Rework other classes to support it.
</commit_message>
<xml_diff>
--- a/data/railway_links.xlsx
+++ b/data/railway_links.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="149">
   <si>
     <t>81-1001</t>
   </si>
@@ -418,18 +418,12 @@
     <t>1-1003</t>
   </si>
   <si>
-    <t>3-12</t>
-  </si>
-  <si>
     <t>3-1003</t>
   </si>
   <si>
     <t>11-1011</t>
   </si>
   <si>
-    <t>12-1012</t>
-  </si>
-  <si>
     <t>17-1011</t>
   </si>
   <si>
@@ -446,6 +440,27 @@
   </si>
   <si>
     <t>gauge</t>
+  </si>
+  <si>
+    <t>3-13</t>
+  </si>
+  <si>
+    <t>13-1012</t>
+  </si>
+  <si>
+    <t>27-51</t>
+  </si>
+  <si>
+    <t>35-44</t>
+  </si>
+  <si>
+    <t>68-69</t>
+  </si>
+  <si>
+    <t>69-70</t>
+  </si>
+  <si>
+    <t>49-1023</t>
   </si>
 </sst>
 </file>
@@ -798,7 +813,7 @@
   <dimension ref="A1:C215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2:C148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +830,7 @@
         <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -826,7 +841,7 @@
         <v>94.8</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,7 +852,7 @@
         <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,7 +863,7 @@
         <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,7 +874,7 @@
         <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,7 +885,7 @@
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,7 +896,7 @@
         <v>114</v>
       </c>
       <c r="C7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,7 +907,7 @@
         <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -903,7 +918,7 @@
         <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -914,7 +929,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -925,7 +940,7 @@
         <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,7 +951,7 @@
         <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,7 +962,7 @@
         <v>115</v>
       </c>
       <c r="C13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,7 +973,7 @@
         <v>84</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -969,7 +984,7 @@
         <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,7 +995,7 @@
         <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,7 +1006,7 @@
         <v>161</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,7 +1017,7 @@
         <v>200</v>
       </c>
       <c r="C18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,7 +1028,7 @@
         <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,7 +1039,7 @@
         <v>172</v>
       </c>
       <c r="C20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,7 +1050,7 @@
         <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,7 +1061,7 @@
         <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1072,7 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1068,7 +1083,7 @@
         <v>58.2</v>
       </c>
       <c r="C24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,7 +1094,7 @@
         <v>69.900000000000006</v>
       </c>
       <c r="C25" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,7 +1105,7 @@
         <v>166</v>
       </c>
       <c r="C26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,7 +1116,7 @@
         <v>228</v>
       </c>
       <c r="C27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,7 +1127,7 @@
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,7 +1138,7 @@
         <v>146</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,7 +1149,7 @@
         <v>93.2</v>
       </c>
       <c r="C30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,7 +1160,7 @@
         <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,7 +1171,7 @@
         <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,7 +1182,7 @@
         <v>68</v>
       </c>
       <c r="C33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,7 +1193,7 @@
         <v>55.6</v>
       </c>
       <c r="C34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1189,7 +1204,7 @@
         <v>169</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1200,7 +1215,7 @@
         <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1211,7 +1226,7 @@
         <v>60</v>
       </c>
       <c r="C37" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1222,7 +1237,7 @@
         <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1233,7 +1248,7 @@
         <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1244,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1255,7 +1270,7 @@
         <v>82.6</v>
       </c>
       <c r="C41" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1266,7 +1281,7 @@
         <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1277,7 +1292,7 @@
         <v>140</v>
       </c>
       <c r="C43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1288,7 +1303,7 @@
         <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1299,7 +1314,7 @@
         <v>131</v>
       </c>
       <c r="C45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1310,7 +1325,7 @@
         <v>230</v>
       </c>
       <c r="C46" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1321,7 +1336,7 @@
         <v>301</v>
       </c>
       <c r="C47" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1332,7 +1347,7 @@
         <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1343,7 +1358,7 @@
         <v>202</v>
       </c>
       <c r="C49" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1354,7 +1369,7 @@
         <v>208</v>
       </c>
       <c r="C50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1365,7 +1380,7 @@
         <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1376,7 +1391,7 @@
         <v>125</v>
       </c>
       <c r="C52" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,7 +1402,7 @@
         <v>64</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1398,7 +1413,7 @@
         <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1409,7 +1424,7 @@
         <v>164</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1420,7 +1435,7 @@
         <v>175</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1431,7 +1446,7 @@
         <v>129</v>
       </c>
       <c r="C57" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1442,7 +1457,7 @@
         <v>125</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1453,7 +1468,7 @@
         <v>100</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1464,7 +1479,7 @@
         <v>97.7</v>
       </c>
       <c r="C60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1475,7 +1490,7 @@
         <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1486,7 +1501,7 @@
         <v>80</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,7 +1512,7 @@
         <v>100</v>
       </c>
       <c r="C63" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,7 +1523,7 @@
         <v>175</v>
       </c>
       <c r="C64" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1519,7 +1534,7 @@
         <v>280</v>
       </c>
       <c r="C65" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1530,7 +1545,7 @@
         <v>109</v>
       </c>
       <c r="C66" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1541,7 +1556,7 @@
         <v>94</v>
       </c>
       <c r="C67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,7 +1567,7 @@
         <v>60</v>
       </c>
       <c r="C68" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,7 +1578,7 @@
         <v>366</v>
       </c>
       <c r="C69" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,7 +1589,7 @@
         <v>181</v>
       </c>
       <c r="C70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1585,7 +1600,7 @@
         <v>148</v>
       </c>
       <c r="C71" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,7 +1611,7 @@
         <v>195</v>
       </c>
       <c r="C72" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,7 +1622,7 @@
         <v>101</v>
       </c>
       <c r="C73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1618,7 +1633,7 @@
         <v>84.8</v>
       </c>
       <c r="C74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1629,7 +1644,7 @@
         <v>150</v>
       </c>
       <c r="C75" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1640,7 +1655,7 @@
         <v>218</v>
       </c>
       <c r="C76" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1651,7 +1666,7 @@
         <v>134</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1662,7 +1677,7 @@
         <v>200</v>
       </c>
       <c r="C78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1673,7 +1688,7 @@
         <v>130</v>
       </c>
       <c r="C79" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,7 +1699,7 @@
         <v>110</v>
       </c>
       <c r="C80" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1695,7 +1710,7 @@
         <v>69.5</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -1706,7 +1721,7 @@
         <v>110</v>
       </c>
       <c r="C82" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -1717,7 +1732,7 @@
         <v>185</v>
       </c>
       <c r="C83" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -1728,7 +1743,7 @@
         <v>161</v>
       </c>
       <c r="C84" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1739,7 +1754,7 @@
         <v>169</v>
       </c>
       <c r="C85" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1750,7 +1765,7 @@
         <v>258</v>
       </c>
       <c r="C86" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1761,7 +1776,7 @@
         <v>99</v>
       </c>
       <c r="C87" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1772,7 +1787,7 @@
         <v>100</v>
       </c>
       <c r="C88" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1783,7 +1798,7 @@
         <v>184</v>
       </c>
       <c r="C89" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1794,7 +1809,7 @@
         <v>440</v>
       </c>
       <c r="C90" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,7 +1820,7 @@
         <v>195</v>
       </c>
       <c r="C91" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1816,7 +1831,7 @@
         <v>47</v>
       </c>
       <c r="C92" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1827,7 +1842,7 @@
         <v>56</v>
       </c>
       <c r="C93" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,7 +1853,7 @@
         <v>70</v>
       </c>
       <c r="C94" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,7 +1864,7 @@
         <v>64</v>
       </c>
       <c r="C95" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,524 +1875,579 @@
         <v>110</v>
       </c>
       <c r="C96" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B97">
-        <v>185</v>
+        <v>308</v>
       </c>
       <c r="C97" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="B98">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C98" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>56</v>
+        <v>148</v>
       </c>
       <c r="B99">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="C99" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B100">
-        <v>340</v>
+        <v>185</v>
       </c>
       <c r="C100" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="B101">
-        <v>95</v>
+        <v>225</v>
       </c>
       <c r="C101" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B102">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C102" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>127</v>
+        <v>86</v>
       </c>
       <c r="B103">
-        <v>240</v>
+        <v>340</v>
       </c>
       <c r="C103" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>128</v>
+        <v>23</v>
       </c>
       <c r="B104">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="C104" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B105">
-        <v>123</v>
+        <v>172</v>
       </c>
       <c r="C105" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="B106">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="C106" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="B107">
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="C107" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="B108">
-        <v>208</v>
+        <v>123</v>
       </c>
       <c r="C108" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B109">
-        <v>360</v>
+        <v>221</v>
       </c>
       <c r="C109" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B110">
-        <v>148</v>
+        <v>250</v>
       </c>
       <c r="C110" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B111">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="C111" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="B112">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="C112" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>130</v>
+        <v>52</v>
       </c>
       <c r="B113">
-        <v>493</v>
+        <v>148</v>
       </c>
       <c r="C113" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="B114">
-        <v>262</v>
+        <v>116</v>
       </c>
       <c r="C114" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B115">
-        <v>182</v>
+        <v>260</v>
       </c>
       <c r="C115" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="B116">
-        <v>298</v>
+        <v>493</v>
       </c>
       <c r="C116" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B117">
-        <v>453</v>
+        <v>262</v>
       </c>
       <c r="C117" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B118">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C118" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="B119">
-        <v>493</v>
+        <v>298</v>
       </c>
       <c r="C119" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B120">
-        <v>166</v>
+        <v>453</v>
       </c>
       <c r="C120" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B121">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="C121" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="B122">
-        <v>80</v>
+        <v>493</v>
       </c>
       <c r="C122" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B123">
-        <v>36</v>
+        <v>166</v>
       </c>
       <c r="C123" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>2</v>
+        <v>132</v>
       </c>
       <c r="B124">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="C124" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B125">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C125" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="B126">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="C126" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B127">
-        <v>216</v>
+        <v>50</v>
       </c>
       <c r="C127" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="B128">
-        <v>169</v>
+        <v>98</v>
       </c>
       <c r="C128" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>97</v>
+        <v>31</v>
       </c>
       <c r="B129">
-        <v>94.8</v>
+        <v>70</v>
       </c>
       <c r="C129" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>133</v>
+        <v>74</v>
       </c>
       <c r="B130">
-        <v>58</v>
+        <v>216</v>
       </c>
       <c r="C130" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="B131">
-        <v>250</v>
+        <v>169</v>
       </c>
       <c r="C131" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="B132">
-        <v>45</v>
+        <v>94.8</v>
       </c>
       <c r="C132" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B133">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="C133" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B134">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="C134" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="B135">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="C135" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B136">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C136" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="B137">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="C137" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>137</v>
+        <v>38</v>
       </c>
       <c r="B138">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C138" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="B139">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="C139" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="B140">
-        <v>199</v>
+        <v>66</v>
       </c>
       <c r="C140" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B141">
-        <v>340</v>
+        <v>60</v>
       </c>
       <c r="C141" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="B142">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="C142" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B143">
+        <v>199</v>
+      </c>
+      <c r="C143" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B144">
+        <v>340</v>
+      </c>
+      <c r="C144" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B145">
+        <v>80</v>
+      </c>
+      <c r="C145" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B143">
+      <c r="B146">
         <v>353</v>
       </c>
-      <c r="C143" t="s">
-        <v>142</v>
+      <c r="C146" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>245</v>
+      </c>
+      <c r="C147" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>210</v>
+      </c>
+      <c r="C148" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rework methods and classes to add global results report.
</commit_message>
<xml_diff>
--- a/data/railway_links.xlsx
+++ b/data/railway_links.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="150">
   <si>
     <t>81-1001</t>
   </si>
@@ -409,9 +409,6 @@
     <t>66-77</t>
   </si>
   <si>
-    <t>78-79</t>
-  </si>
-  <si>
     <t>78-1001</t>
   </si>
   <si>
@@ -461,6 +458,12 @@
   </si>
   <si>
     <t>49-1023</t>
+  </si>
+  <si>
+    <t>78-1079</t>
+  </si>
+  <si>
+    <t>79-1079</t>
   </si>
 </sst>
 </file>
@@ -812,14 +815,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C148"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,150 +832,150 @@
         <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="B2">
-        <v>94.8</v>
+        <v>440</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B3">
-        <v>129</v>
+        <v>366</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>101</v>
+        <v>143</v>
       </c>
       <c r="B4">
-        <v>105</v>
+        <v>308</v>
       </c>
       <c r="C4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B5">
-        <v>103</v>
+        <v>230</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>214</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B7">
-        <v>114</v>
+        <v>208</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="B9">
-        <v>76</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
       <c r="B10">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B12">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B13">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B14">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,84 +986,84 @@
         <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="B16">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="B17">
-        <v>161</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>200</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>118</v>
       </c>
       <c r="B19">
-        <v>158</v>
+        <v>100</v>
       </c>
       <c r="C19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B20">
-        <v>172</v>
+        <v>100</v>
       </c>
       <c r="C20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="B21">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B22">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,51 +1074,51 @@
         <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="B24">
-        <v>58.2</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>69.900000000000006</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B26">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>228</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1127,865 +1129,865 @@
         <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>50</v>
+        <v>125</v>
       </c>
       <c r="B29">
-        <v>146</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B30">
-        <v>93.2</v>
+        <v>47</v>
       </c>
       <c r="C30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>21</v>
+        <v>102</v>
       </c>
       <c r="B32">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="B33">
-        <v>68</v>
+        <v>94.8</v>
       </c>
       <c r="C33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>3</v>
+        <v>71</v>
       </c>
       <c r="B34">
-        <v>55.6</v>
+        <v>200</v>
       </c>
       <c r="C34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B35">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B36">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="B37">
-        <v>60</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B38">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B39">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="C39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="B40">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B41">
-        <v>82.6</v>
+        <v>142</v>
       </c>
       <c r="C41" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="B42">
-        <v>169</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B43">
-        <v>140</v>
+        <v>58.2</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="B44">
-        <v>151</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="C44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B45">
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>111</v>
+        <v>78</v>
       </c>
       <c r="B46">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B47">
-        <v>301</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B48">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="B49">
-        <v>202</v>
+        <v>93.2</v>
       </c>
       <c r="C49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="B50">
-        <v>208</v>
+        <v>90</v>
       </c>
       <c r="C50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>114</v>
+        <v>50</v>
       </c>
       <c r="B51">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="B52">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B53">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B54">
-        <v>154</v>
+        <v>55.6</v>
       </c>
       <c r="C54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="B55">
-        <v>164</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
       <c r="B56">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B57">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B58">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B59">
-        <v>100</v>
+        <v>82.6</v>
       </c>
       <c r="C59" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B60">
-        <v>97.7</v>
+        <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B61">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
       <c r="B62">
-        <v>80</v>
+        <v>151</v>
       </c>
       <c r="C62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>118</v>
+        <v>44</v>
       </c>
       <c r="B63">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="B64">
-        <v>175</v>
+        <v>301</v>
       </c>
       <c r="C64" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B65">
-        <v>280</v>
+        <v>202</v>
       </c>
       <c r="C65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B66">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B67">
-        <v>94</v>
+        <v>154</v>
       </c>
       <c r="C67" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B68">
-        <v>60</v>
+        <v>164</v>
       </c>
       <c r="C68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>120</v>
+        <v>42</v>
       </c>
       <c r="B69">
-        <v>366</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="B70">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="C70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="B71">
-        <v>148</v>
+        <v>50</v>
       </c>
       <c r="C71" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="B72">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B73">
-        <v>101</v>
+        <v>97.7</v>
       </c>
       <c r="C73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B74">
-        <v>84.8</v>
+        <v>123</v>
       </c>
       <c r="C74" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B75">
-        <v>150</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B76">
-        <v>218</v>
+        <v>109</v>
       </c>
       <c r="C76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B77">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="C77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="B78">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="C78" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B79">
-        <v>130</v>
+        <v>60</v>
       </c>
       <c r="C79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B80">
-        <v>110</v>
+        <v>181</v>
       </c>
       <c r="C80" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="B81">
-        <v>69.5</v>
+        <v>170</v>
       </c>
       <c r="C81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B82">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="C82" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="B83">
-        <v>185</v>
+        <v>101</v>
       </c>
       <c r="C83" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="B84">
-        <v>161</v>
+        <v>84.8</v>
       </c>
       <c r="C84" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B85">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C85" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B86">
-        <v>258</v>
+        <v>218</v>
       </c>
       <c r="C86" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="B87">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="C87" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B88">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C88" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B89">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="C89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="B90">
-        <v>440</v>
+        <v>69.5</v>
       </c>
       <c r="C90" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>124</v>
+        <v>69</v>
       </c>
       <c r="B91">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C91" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="B92">
-        <v>47</v>
+        <v>161</v>
       </c>
       <c r="C92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="B93">
-        <v>56</v>
+        <v>115</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B94">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B95">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="C95" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="B96">
-        <v>110</v>
+        <v>258</v>
       </c>
       <c r="C96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="B97">
-        <v>308</v>
+        <v>72</v>
       </c>
       <c r="C97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>145</v>
+        <v>27</v>
       </c>
       <c r="B98">
-        <v>214</v>
+        <v>99</v>
       </c>
       <c r="C98" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="B99">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C99" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="B100">
-        <v>185</v>
+        <v>212</v>
       </c>
       <c r="C100" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>77</v>
+        <v>4</v>
       </c>
       <c r="B101">
-        <v>225</v>
+        <v>40</v>
       </c>
       <c r="C101" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="B102">
-        <v>158</v>
+        <v>493</v>
       </c>
       <c r="C102" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>86</v>
+        <v>129</v>
       </c>
       <c r="B103">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="C103" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>23</v>
+        <v>127</v>
       </c>
       <c r="B104">
-        <v>95</v>
+        <v>240</v>
       </c>
       <c r="C104" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>64</v>
+        <v>126</v>
       </c>
       <c r="B105">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C105" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B106">
-        <v>240</v>
+        <v>142</v>
       </c>
       <c r="C106" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -1996,227 +1998,227 @@
         <v>120</v>
       </c>
       <c r="C107" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B108">
-        <v>123</v>
+        <v>225</v>
       </c>
       <c r="C108" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B109">
-        <v>221</v>
+        <v>158</v>
       </c>
       <c r="C109" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B110">
-        <v>250</v>
+        <v>340</v>
       </c>
       <c r="C110" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="B111">
-        <v>208</v>
+        <v>95</v>
       </c>
       <c r="C111" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>129</v>
+        <v>64</v>
       </c>
       <c r="B112">
-        <v>360</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B113">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="C113" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B114">
-        <v>116</v>
+        <v>221</v>
       </c>
       <c r="C114" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B115">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C115" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="B116">
-        <v>493</v>
+        <v>208</v>
       </c>
       <c r="C116" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B117">
-        <v>262</v>
+        <v>148</v>
       </c>
       <c r="C117" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="B118">
-        <v>182</v>
+        <v>116</v>
       </c>
       <c r="C118" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B119">
-        <v>298</v>
+        <v>260</v>
       </c>
       <c r="C119" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B120">
-        <v>453</v>
+        <v>262</v>
       </c>
       <c r="C120" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B121">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="C121" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="B122">
-        <v>493</v>
+        <v>298</v>
       </c>
       <c r="C122" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B123">
-        <v>166</v>
+        <v>453</v>
       </c>
       <c r="C123" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>132</v>
+        <v>70</v>
       </c>
       <c r="B124">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="C124" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="B125">
-        <v>80</v>
+        <v>166</v>
       </c>
       <c r="C125" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B126">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="C126" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B127">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C127" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -2227,227 +2229,249 @@
         <v>98</v>
       </c>
       <c r="C128" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="B129">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C129" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B130">
-        <v>216</v>
+        <v>70</v>
       </c>
       <c r="C130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B131">
-        <v>169</v>
+        <v>216</v>
       </c>
       <c r="C131" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B132">
-        <v>94.8</v>
+        <v>169</v>
       </c>
       <c r="C132" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="B133">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="C133" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B134">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="C134" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B135">
-        <v>45</v>
+        <v>340</v>
       </c>
       <c r="C135" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>99</v>
+        <v>141</v>
       </c>
       <c r="B136">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="C136" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B137">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="C137" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="B138">
-        <v>120</v>
+        <v>58</v>
       </c>
       <c r="C138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>90</v>
+        <v>133</v>
       </c>
       <c r="B139">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C139" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="B140">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="C140" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>143</v>
+        <v>38</v>
       </c>
       <c r="B141">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="C141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="B142">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="B143">
-        <v>199</v>
+        <v>60</v>
       </c>
       <c r="C143" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
       <c r="B144">
-        <v>340</v>
+        <v>66</v>
       </c>
       <c r="C144" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>14</v>
+        <v>135</v>
       </c>
       <c r="B145">
-        <v>80</v>
+        <v>199</v>
       </c>
       <c r="C145" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="B146">
-        <v>353</v>
+        <v>114</v>
       </c>
       <c r="C146" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147">
         <v>245</v>
       </c>
       <c r="C147" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>210</v>
       </c>
       <c r="C148" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B149">
+        <v>80</v>
+      </c>
+      <c r="C149" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B150">
+        <v>353</v>
+      </c>
+      <c r="C150" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix minor bugs and change data.
</commit_message>
<xml_diff>
--- a/data/railway_links.xlsx
+++ b/data/railway_links.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="151">
   <si>
     <t>81-1001</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>79-1079</t>
+  </si>
+  <si>
+    <t>29-49</t>
   </si>
 </sst>
 </file>
@@ -815,7 +818,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C215"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2474,6 +2479,17 @@
         <v>139</v>
       </c>
     </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>141</v>
+      </c>
+      <c r="C151" t="s">
+        <v>137</v>
+      </c>
+    </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="3"/>

</xml_diff>

<commit_message>
Changes in derivation coefficient calculation and derivation criteria. Changes in data. Fix some bugs in dijkstra subpackage. Individual find_shortest_path called from modal_networks is not working properly, it needs to be revised. At this point data is enough to not use that method anyway.
</commit_message>
<xml_diff>
--- a/data/railway_links.xlsx
+++ b/data/railway_links.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="149">
   <si>
     <t>81-1001</t>
   </si>
@@ -337,9 +337,6 @@
     <t>id_link</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
     <t>7-26</t>
   </si>
   <si>
@@ -403,9 +400,6 @@
     <t>21-1021</t>
   </si>
   <si>
-    <t>63-67</t>
-  </si>
-  <si>
     <t>66-77</t>
   </si>
   <si>
@@ -448,9 +442,6 @@
     <t>27-51</t>
   </si>
   <si>
-    <t>35-44</t>
-  </si>
-  <si>
     <t>68-69</t>
   </si>
   <si>
@@ -467,13 +458,16 @@
   </si>
   <si>
     <t>29-49</t>
+  </si>
+  <si>
+    <t>dist</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -485,6 +479,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -510,11 +512,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C215"/>
+  <dimension ref="A1:C214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,66 +834,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" t="s">
-        <v>140</v>
+      <c r="B1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>440</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B3">
-        <v>366</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B4">
-        <v>308</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B5">
-        <v>230</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="B6">
-        <v>214</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>137</v>
@@ -897,21 +901,21 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B7">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B8">
-        <v>200</v>
+        <v>108</v>
       </c>
       <c r="C8" t="s">
         <v>137</v>
@@ -919,10 +923,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>38</v>
       </c>
       <c r="B9">
-        <v>195</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>137</v>
@@ -930,10 +934,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B10">
-        <v>195</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>137</v>
@@ -941,10 +945,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B11">
-        <v>175</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>137</v>
@@ -952,10 +956,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="B12">
-        <v>141</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
         <v>137</v>
@@ -963,21 +967,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B13">
-        <v>126</v>
+        <v>94.8</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="B14">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>137</v>
@@ -985,87 +989,87 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B15">
-        <v>122</v>
+        <v>225</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="B16">
-        <v>117</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B17">
-        <v>110</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B18">
-        <v>110</v>
+        <v>340</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B21">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="B22">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="C22" t="s">
         <v>137</v>
@@ -1073,10 +1077,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>109</v>
+        <v>35</v>
       </c>
       <c r="B23">
-        <v>82</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
         <v>137</v>
@@ -1084,373 +1088,373 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>117</v>
+        <v>64</v>
       </c>
       <c r="B24">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="B25">
-        <v>70</v>
+        <v>172</v>
       </c>
       <c r="C25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="B26">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="B27">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>108</v>
       </c>
       <c r="B28">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>125</v>
+        <v>48</v>
       </c>
       <c r="B29">
-        <v>56</v>
+        <v>142</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B30">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="B31">
-        <v>161</v>
+        <v>58.2</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="B32">
-        <v>114</v>
+        <v>240</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="B33">
-        <v>94.8</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="B34">
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B35">
-        <v>158</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="B36">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="C36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="B37">
-        <v>105</v>
+        <v>228</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
         <v>64</v>
       </c>
-      <c r="B38">
-        <v>172</v>
-      </c>
       <c r="C38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="B39">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B40">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C40" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B41">
-        <v>142</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B42">
-        <v>74</v>
+        <v>93.2</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B43">
-        <v>58.2</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B44">
-        <v>69.900000000000006</v>
+        <v>146</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B45">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="B46">
-        <v>228</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B47">
-        <v>76</v>
+        <v>169</v>
       </c>
       <c r="C47" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>95</v>
+        <v>3</v>
       </c>
       <c r="B48">
-        <v>80</v>
+        <v>55.6</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
       <c r="B49">
-        <v>93.2</v>
+        <v>141</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B50">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>141</v>
       </c>
       <c r="B51">
-        <v>146</v>
+        <v>308</v>
       </c>
       <c r="C51" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B53">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>3</v>
+        <v>147</v>
       </c>
       <c r="B54">
-        <v>55.6</v>
+        <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B55">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="C55" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="B56">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="C56" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>16</v>
+        <v>131</v>
       </c>
       <c r="B57">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="C57" t="s">
         <v>137</v>
@@ -1458,21 +1462,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B58">
-        <v>102</v>
+        <v>82.6</v>
       </c>
       <c r="C58" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>17</v>
+        <v>139</v>
       </c>
       <c r="B59">
-        <v>82.6</v>
+        <v>250</v>
       </c>
       <c r="C59" t="s">
         <v>137</v>
@@ -1486,7 +1490,7 @@
         <v>169</v>
       </c>
       <c r="C60" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1497,7 +1501,7 @@
         <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1508,994 +1512,950 @@
         <v>151</v>
       </c>
       <c r="C62" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="B63">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>85</v>
+        <v>44</v>
       </c>
       <c r="B64">
-        <v>301</v>
+        <v>131</v>
       </c>
       <c r="C64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="B65">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="C65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="B66">
-        <v>64</v>
+        <v>301</v>
       </c>
       <c r="C66" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="B67">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="C67" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>58</v>
+        <v>114</v>
       </c>
       <c r="B68">
-        <v>164</v>
+        <v>125</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B69">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B70">
-        <v>125</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="B71">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B72">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="C72" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B73">
-        <v>97.7</v>
+        <v>164</v>
       </c>
       <c r="C73" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="B74">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="B75">
-        <v>69</v>
+        <v>129</v>
       </c>
       <c r="C75" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B76">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B77">
-        <v>175</v>
+        <v>50</v>
       </c>
       <c r="C77" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>83</v>
+        <v>28</v>
       </c>
       <c r="B78">
-        <v>280</v>
+        <v>100</v>
       </c>
       <c r="C78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B79">
-        <v>60</v>
+        <v>97.7</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="B80">
-        <v>181</v>
+        <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="B81">
-        <v>170</v>
+        <v>123</v>
       </c>
       <c r="C81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>51</v>
+        <v>116</v>
       </c>
       <c r="B82">
-        <v>148</v>
+        <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
       <c r="B83">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B84">
-        <v>84.8</v>
+        <v>109</v>
       </c>
       <c r="C84" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B85">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="C85" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B86">
-        <v>218</v>
+        <v>280</v>
       </c>
       <c r="C86" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="B87">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="C87" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B88">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="C88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="B89">
-        <v>130</v>
+        <v>366</v>
       </c>
       <c r="C89" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B90">
-        <v>69.5</v>
+        <v>181</v>
       </c>
       <c r="C90" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>69</v>
+        <v>144</v>
       </c>
       <c r="B91">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C91" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B92">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="C92" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="B93">
-        <v>115</v>
+        <v>195</v>
       </c>
       <c r="C93" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B94">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C94" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="B95">
-        <v>169</v>
+        <v>84.8</v>
       </c>
       <c r="C95" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="B96">
-        <v>258</v>
+        <v>123</v>
       </c>
       <c r="C96" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B97">
-        <v>72</v>
+        <v>221</v>
       </c>
       <c r="C97" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="B98">
-        <v>99</v>
+        <v>250</v>
       </c>
       <c r="C98" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B99">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="C99" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>144</v>
+        <v>53</v>
       </c>
       <c r="B100">
-        <v>212</v>
+        <v>150</v>
       </c>
       <c r="C100" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B101">
-        <v>40</v>
+        <v>218</v>
       </c>
       <c r="C101" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="B102">
-        <v>493</v>
+        <v>134</v>
       </c>
       <c r="C102" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="B103">
-        <v>360</v>
+        <v>70</v>
       </c>
       <c r="C103" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
       <c r="B104">
-        <v>240</v>
+        <v>110</v>
       </c>
       <c r="C104" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B105">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C105" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="B106">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C106" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="B107">
-        <v>120</v>
+        <v>69.5</v>
       </c>
       <c r="C107" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>77</v>
+        <v>24</v>
       </c>
       <c r="B108">
-        <v>225</v>
+        <v>110</v>
       </c>
       <c r="C108" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B109">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="C109" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B110">
-        <v>340</v>
+        <v>148</v>
       </c>
       <c r="C110" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B111">
-        <v>95</v>
+        <v>161</v>
       </c>
       <c r="C111" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B112">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="C112" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B113">
-        <v>123</v>
+        <v>260</v>
       </c>
       <c r="C113" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
       <c r="B114">
-        <v>221</v>
+        <v>493</v>
       </c>
       <c r="C114" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B115">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="C115" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B116">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="C116" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="B117">
-        <v>148</v>
+        <v>245</v>
       </c>
       <c r="C117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="B118">
-        <v>116</v>
+        <v>340</v>
       </c>
       <c r="C118" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B119">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="C119" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="B120">
-        <v>262</v>
+        <v>80</v>
       </c>
       <c r="C120" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="B121">
-        <v>182</v>
+        <v>353</v>
       </c>
       <c r="C121" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B122">
-        <v>298</v>
+        <v>117</v>
       </c>
       <c r="C122" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B123">
-        <v>453</v>
+        <v>115</v>
       </c>
       <c r="C123" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B124">
-        <v>196</v>
+        <v>298</v>
       </c>
       <c r="C124" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B125">
-        <v>166</v>
+        <v>453</v>
       </c>
       <c r="C125" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="B126">
-        <v>80</v>
+        <v>196</v>
       </c>
       <c r="C126" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="B127">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="C127" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>26</v>
+        <v>145</v>
       </c>
       <c r="B128">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C128" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="B129">
-        <v>50</v>
+        <v>166</v>
       </c>
       <c r="C129" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="B130">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C130" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="B131">
-        <v>216</v>
+        <v>80</v>
       </c>
       <c r="C131" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B132">
-        <v>169</v>
+        <v>122</v>
       </c>
       <c r="C132" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>148</v>
+        <v>0</v>
       </c>
       <c r="B133">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="C133" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="B134">
-        <v>50</v>
+        <v>98</v>
       </c>
       <c r="C134" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="B135">
-        <v>340</v>
+        <v>84</v>
       </c>
       <c r="C135" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>141</v>
+        <v>2</v>
       </c>
       <c r="B136">
-        <v>250</v>
+        <v>50</v>
       </c>
       <c r="C136" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="B137">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C137" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>132</v>
+        <v>74</v>
       </c>
       <c r="B138">
-        <v>58</v>
+        <v>216</v>
       </c>
       <c r="C138" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>133</v>
+        <v>63</v>
       </c>
       <c r="B139">
-        <v>45</v>
+        <v>169</v>
       </c>
       <c r="C139" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="B140">
-        <v>108</v>
+        <v>169</v>
       </c>
       <c r="C140" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="B141">
-        <v>120</v>
+        <v>258</v>
       </c>
       <c r="C141" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B142">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C142" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="B143">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C143" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="B144">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="C144" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>135</v>
+        <v>68</v>
       </c>
       <c r="B145">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C145" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="B146">
-        <v>114</v>
+        <v>440</v>
       </c>
       <c r="C146" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B147">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="C147" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B148">
-        <v>210</v>
-      </c>
-      <c r="C148" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B149">
-        <v>80</v>
-      </c>
-      <c r="C149" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B150">
-        <v>353</v>
-      </c>
-      <c r="C150" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B151">
-        <v>141</v>
-      </c>
-      <c r="C151" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A215" s="2"/>
-      <c r="B215" s="3"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="2"/>
+      <c r="B214" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>